<commit_message>
DDLS-639 Small logic changes to processing and test fixes
</commit_message>
<xml_diff>
--- a/serve-web/tests/TestData/remove_cases.xlsx
+++ b/serve-web/tests/TestData/remove_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.rafferty/GitHub/serve-opg/serve-web/tests/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF9B001A-BC0E-5849-8CA5-27EE4E7443A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D33D6A-2E32-864E-862A-0330D4B03905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36420" yWindow="1380" windowWidth="34560" windowHeight="19540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="3560" windowWidth="34560" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="remove_cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Case number</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Order Issue Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Court order </t>
-  </si>
-  <si>
     <t>BOBBY FISHER</t>
   </si>
   <si>
@@ -44,6 +41,15 @@
   </si>
   <si>
     <t>SHERRIE MCARTHUR</t>
+  </si>
+  <si>
+    <t>Court order</t>
+  </si>
+  <si>
+    <t>CHARLIE THOMPSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEE OSWARLD </t>
   </si>
 </sst>
 </file>
@@ -307,10 +313,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -324,8 +330,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -345,7 +351,7 @@
         <v>40002001</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>45497</v>
@@ -362,7 +368,7 @@
         <v>40002002</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
         <v>45510</v>
@@ -379,7 +385,7 @@
         <v>40002003</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1">
         <v>45521</v>
@@ -390,18 +396,35 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>11052088</v>
+        <v>11052066</v>
       </c>
       <c r="B5">
-        <v>40002005</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>45521</v>
       </c>
       <c r="E5" s="1">
+        <v>45579</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>11052077</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45521</v>
+      </c>
+      <c r="E6" s="1">
         <v>45579</v>
       </c>
     </row>

</xml_diff>